<commit_message>
Swapped formats to the proper ones
</commit_message>
<xml_diff>
--- a/statistics/documents/exampleFormat0.xlsx
+++ b/statistics/documents/exampleFormat0.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\vesterlund\chalmers-course-stats\statistics\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5E8E41-2735-45E0-8039-2206D2843CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC80974E-A58B-4156-9AD6-CF803FAF7F45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30675" yWindow="1440" windowWidth="23580" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="1530" windowWidth="23580" windowHeight="13215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Beksrivning" sheetId="1" r:id="rId1"/>
-    <sheet name="Läsår 20xx_20yy" sheetId="2" r:id="rId2"/>
-    <sheet name="Läsår 20zz-20aa" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Kurs</t>
   </si>
@@ -78,28 +76,14 @@
   </si>
   <si>
     <t>U</t>
-  </si>
-  <si>
-    <t>Exempeldoukument för format 0</t>
-  </si>
-  <si>
-    <t>Kan ha godtyckligt många läsår som följer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -117,17 +101,6 @@
       <color indexed="63"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -185,26 +158,24 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{D1B89E50-AA65-410A-A45A-3E558A3B7F8A}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{7F0BADC9-17BB-40FE-AC71-D9E0B0A57DD1}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -482,88 +453,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075D4D67-21E0-4C02-9A98-2796867ED2AF}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="42" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -589,7 +524,7 @@
       <c r="G2">
         <v>7.5</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="4">
         <v>44239</v>
       </c>
       <c r="I2" t="s">
@@ -624,7 +559,7 @@
       <c r="G3">
         <v>7.5</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>44239</v>
       </c>
       <c r="I3">
@@ -659,7 +594,7 @@
       <c r="G4">
         <v>7.5</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>44239</v>
       </c>
       <c r="I4">
@@ -694,206 +629,8 @@
       <c r="G5">
         <v>7.5</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>44239</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1916754-5C90-4B0B-AB2A-4DD6E816661A}">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2">
-        <v>109</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>7.5</v>
-      </c>
-      <c r="H2" s="6">
-        <v>44676</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2">
-        <v>95</v>
-      </c>
-      <c r="K2">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>109</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>7.5</v>
-      </c>
-      <c r="H3" s="6">
-        <v>44676</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>109</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4">
-        <v>7.5</v>
-      </c>
-      <c r="H4" s="6">
-        <v>44676</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>109</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5">
-        <v>7.5</v>
-      </c>
-      <c r="H5" s="6">
-        <v>44676</v>
       </c>
       <c r="I5">
         <v>5</v>

</xml_diff>